<commit_message>
Ticket 56 - Fix crash on if tag processing if a font in the rich text string attribute has the color "automatic" in the Excel template.  Have SheetUtil's setCellValue use the CellStyleCache and the FontCache if it needs to set the CellStyle.
</commit_message>
<xml_diff>
--- a/jett-core/templates/IfTagTemplate.xlsx
+++ b/jett-core/templates/IfTagTemplate.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="96">
   <si>
     <t>If Tag Testing</t>
   </si>
@@ -383,12 +383,57 @@
       <t>/&gt;</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>&lt;jt:if test="${num &lt; 5}" then="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>${num}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" else="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>${num}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" /&gt;</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -426,6 +471,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1034,16 +1086,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D10:E10"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1564,11 +1616,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E8"/>
-    <mergeCell ref="D10:E10"/>
     <mergeCell ref="B28:C29"/>
     <mergeCell ref="B32:C33"/>
     <mergeCell ref="B36:C37"/>
@@ -1577,6 +1624,11 @@
     <mergeCell ref="D15:E16"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E20"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E8"/>
+    <mergeCell ref="D10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1644,7 +1696,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1660,6 +1712,11 @@
         <v>94</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>